<commit_message>
Actualized Data With Hotel 1D
</commit_message>
<xml_diff>
--- a/Data/habitacionesDatah1.xlsx
+++ b/Data/habitacionesDatah1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegarcia/Desktop/Rockstars/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegarcia/Desktop/Rockstars/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{469B88A2-8DB1-B648-9727-5431959A8714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4054BAAE-A215-2647-8657-7691AA627733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E955423F-AA58-ED46-A17F-96122CEE6861}"/>
+    <workbookView xWindow="12860" yWindow="5040" windowWidth="15940" windowHeight="10980" xr2:uid="{E955423F-AA58-ED46-A17F-96122CEE6861}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,10 +418,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -439,10 +443,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>101</v>
+        <v>10001101</v>
       </c>
       <c r="B2">
-        <v>10101</v>
+        <v>1000110101</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -453,10 +457,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>102</v>
+        <v>10001102</v>
       </c>
       <c r="B3">
-        <v>10102</v>
+        <v>1000110102</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -467,10 +471,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>103</v>
+        <v>10001103</v>
       </c>
       <c r="B4">
-        <v>10103</v>
+        <v>1000110103</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -481,10 +485,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>104</v>
+        <v>10001104</v>
       </c>
       <c r="B5">
-        <v>10104</v>
+        <v>1000110104</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -495,10 +499,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>105</v>
+        <v>10001105</v>
       </c>
       <c r="B6">
-        <v>10105</v>
+        <v>1000110105</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -509,10 +513,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>106</v>
+        <v>10001106</v>
       </c>
       <c r="B7">
-        <v>10106</v>
+        <v>1000110106</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -523,10 +527,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>107</v>
+        <v>10001107</v>
       </c>
       <c r="B8">
-        <v>10107</v>
+        <v>1000110107</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -537,10 +541,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>108</v>
+        <v>10001108</v>
       </c>
       <c r="B9">
-        <v>10108</v>
+        <v>1000110108</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -551,10 +555,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>109</v>
+        <v>10001109</v>
       </c>
       <c r="B10">
-        <v>10109</v>
+        <v>1000110109</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -565,10 +569,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>110</v>
+        <v>10001110</v>
       </c>
       <c r="B11">
-        <v>10110</v>
+        <v>1000110110</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>

</xml_diff>